<commit_message>
insercon para periodoinhabil updated
</commit_message>
<xml_diff>
--- a/Datos/periodoinhabil.xlsx
+++ b/Datos/periodoinhabil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC7AABE-C0E0-42A1-BACB-9D640E884988}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70146B87-873A-44CC-B060-818C30CC3EC0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{5C687F13-986D-4358-82FD-E2A7EB9C45C1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>inicio</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>Vacaciones semana santa</t>
+  </si>
+  <si>
+    <t>aplicadocente</t>
+  </si>
+  <si>
+    <t>aplicadocpaee</t>
+  </si>
+  <si>
+    <t>aplicapaee</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>archivoJustif1.jpg</t>
+  </si>
+  <si>
+    <t>archivoJustif2.jpg</t>
+  </si>
+  <si>
+    <t>justificacionarchivo</t>
   </si>
 </sst>
 </file>
@@ -448,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C870CA-9F9B-4CC1-8EE1-43F53925E74F}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +480,13 @@
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -475,10 +499,20 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -491,10 +525,20 @@
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -507,10 +551,20 @@
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -523,10 +577,20 @@
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -539,10 +603,20 @@
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -555,10 +629,20 @@
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -571,10 +655,20 @@
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -587,10 +681,20 @@
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
@@ -603,10 +707,20 @@
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -619,10 +733,20 @@
       <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -630,7 +754,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -638,7 +762,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -646,7 +770,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -654,7 +778,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -662,7 +786,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>

</xml_diff>